<commit_message>
📝 Update API Contract
</commit_message>
<xml_diff>
--- a/API Contract.xlsx
+++ b/API Contract.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12A4137-AEAF-4E96-906D-7EEEF50AAEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0726BDD3-ADF8-4062-A327-45364E6586CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19FA70AF-4B9D-48E0-ABFD-405686D2EC0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19FA70AF-4B9D-48E0-ABFD-405686D2EC0F}"/>
   </bookViews>
   <sheets>
     <sheet name="API Contract" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>Pricing Service</t>
   </si>
   <si>
-    <t>/api/pricing/{flightId}</t>
-  </si>
-  <si>
     <t>date (YYYY-MM-DD) as query param</t>
   </si>
   <si>
@@ -323,6 +320,9 @@
   </si>
   <si>
     <t>Returns all resevations.</t>
+  </si>
+  <si>
+    <t>/api/pricing/{flightId}/{date}</t>
   </si>
 </sst>
 </file>
@@ -1250,9 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6EC04A4-A1B3-4926-A6DE-23F39A2A7D4F}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1290,7 +1288,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -1310,7 +1308,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
@@ -1330,7 +1328,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
@@ -1350,379 +1348,379 @@
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>